<commit_message>
Működik a winforms api :D
</commit_message>
<xml_diff>
--- a/Egyéb/FeladatokBeosztása.xlsx
+++ b/Egyéb/FeladatokBeosztása.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\FINAL_PROJECT\Etterem_vizsgaremek\Cuccok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\FINAL_PROJECT\Etterem_vizsgaremek\Etterem_vizsgaremek\Egyéb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556302AD-5F7B-498D-B2C1-43809D26AB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4649E70A-44F5-405A-9652-BE53A0DA35FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Feladat</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Winforms Design</t>
   </si>
   <si>
-    <t>Vue Design elkezdése</t>
-  </si>
-  <si>
     <t>Vue navbar design</t>
   </si>
   <si>
@@ -94,6 +91,12 @@
   </si>
   <si>
     <t>Jakab Botond, Krausz Márton, Tóth Dániel</t>
+  </si>
+  <si>
+    <t>Tóth Dániel, Jakab Botond</t>
+  </si>
+  <si>
+    <t>Vue navbar létrehoz</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -536,7 +539,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -544,10 +550,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>

</xml_diff>